<commit_message>
testes 15 a 19
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,90 +436,426 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>priority</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>population size</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>number generations</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>threshold fairness difference</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>threshold negative accuracy</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>fairness metric</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>protected attribute</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>solutions</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>learning rate</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>number generations</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>population size</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>priority</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>protected attribute</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>solutions</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>threshold fairness difference</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>threshold negative accuracy</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Equal Opportunity_Race_(10, 0.001)</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
+          <t>Equal Opportunity_Race_(10, 0.1)</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>50</v>
+      </c>
+      <c r="D2" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>Equal Opportunity</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>[[0.0028462616493179146], [0.002590368198518595], [0.00289355495310106], [0.0029096086771784307], [0.004302053804414838], [0.004427622235551442]]</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>10</v>
-      </c>
-      <c r="E2" t="n">
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Race</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>[[-0.8735132217407227, 0.01620968150286095], [-0.8735546469688416, 0.02065927388728539], [-0.8723527789115906, 0.00232416831231963], [-0.8702805638313293, 0.00029621753000153017], [-0.8640225529670715, 0.00021140310901823778]]</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>[[0.0028737239939516388], [0.002971458386903831], [0.0028684319319696016], [0.00374261365951772], [0.003322649616601183]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Equal Opportunity_Race_(10, 10)</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
         <v>50</v>
       </c>
-      <c r="F2" t="n">
+      <c r="D3" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3" t="n">
+        <v>10</v>
+      </c>
+      <c r="F3" t="n">
+        <v>10</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Equal Opportunity</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Race</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>[[-0.8714824318885803, 0.0001000050635474592], [-0.7522483468055725, 0.0], [-0.7522483468055725, 0.0], [-0.7522483468055725, 0.0], [-0.8719383478164673, 0.003046989720998483], [-0.8716482520103455, 0.0007949769608587287], [-0.8737204074859619, 0.02342143906020555], [-0.8714410066604614, 4.430604081229195e-05], [-0.8734303116798401, 0.009865056458554844]]</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>[[0.0017745076722178134], [0.09895409459406464], [0.0936968270797161], [0.0993825068792214], [0.0036615332415286], [0.0019053222938458059], [0.003641574953726978], [0.0034821088280922443], [0.0026614375568086764]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Equalized Odds_Sex_(0.001, 0.001)</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>1</v>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Race</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>[[-0.872269868850708, 0.004886323358144762], [-0.8733888864517212, 0.035553698921464316], [-0.8742177486419678, 0.03949946832751028], [-0.8729329705238342, 0.02185173932857365], [-0.8716482520103455, 9.620740290650076e-05], [-0.8751295208930969, 0.04536052458352313]]</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
-        <v>10</v>
-      </c>
-      <c r="J2" t="n">
+      <c r="C4" t="n">
+        <v>50</v>
+      </c>
+      <c r="D4" t="n">
+        <v>10</v>
+      </c>
+      <c r="E4" t="n">
         <v>0.001</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Equalized Odds</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>[[-0.8265987038612366, 0.02434565725661994], [-0.8366281390190125, 0.02605185671545674], [-0.8205893039703369, 0.00926165248434338], [-0.861991822719574, 0.03561748593405175], [-0.8743835091590881, 0.06744981278407403], [-0.8514236211776733, 0.029490282491716795], [-0.8687471747398376, 0.048114197214148835], [-0.8671308159828186, 0.03816643353082369], [-0.8685813546180725, 0.044599439702429675], [-0.8725599646568298, 0.05690462725140685], [-0.872477114200592, 0.04852629342814105]]</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>[[0.08947120568403436], [0.06863962454533037], [0.08972192871631018], [0.01608495754267763], [0.0030164253919121643], [0.02642312346147711], [0.0037476388128512305], [0.004986735525391881], [0.0030047753910134724], [0.0031146051421806842], [0.002996645218538682]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Equalized Odds_Sex_(0.001, 0.1)</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>50</v>
+      </c>
+      <c r="D5" t="n">
+        <v>10</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Equalized Odds</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>[[-0.8409797549247742, 0.019156886663060965], [-0.8720211982727051, 0.05518519575823929], [-0.8688715100288391, 0.043365337110828385], [-0.8549463152885437, 0.03789376875341892], [-0.8682084083557129, 0.04321708431802043], [-0.873927652835846, 0.07447845338736221], [-0.8671723008155823, 0.042677477071546344], [-0.8717311024665833, 0.0481274292484796], [-0.8742177486419678, 0.07482657548007596], [-0.8735132217407227, 0.05616074002691672], [-0.8726014494895935, 0.05576672373544059], [-0.8738861680030823, 0.0658587667435385]]</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>[[0.06011712596813006], [0.0023875984547754884], [0.001859066934291876], [0.03252023115285509], [0.009259553645886206], [0.004570539122095032], [0.0026936556435444344], [0.0031369506917890535], [0.002748609887659027], [0.004064160090213528], [0.004228466779856352], [0.004137777386298756]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Equalized Odds_Sex_(0.001, 10)</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>50</v>
+      </c>
+      <c r="D6" t="n">
+        <v>10</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Equalized Odds</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>[[-0.7573459148406982, 0.0], [-0.8416428565979004, 0.02097208002178849], [-0.8485639691352844, 0.03869590779085207], [-0.8467819094657898, 0.02719901879771859], [-0.8742591738700867, 0.05169646510510659], [-0.8656388521194458, 0.03961320024658648], [-0.8704878091812134, 0.05025764532541417], [-0.8675453066825867, 0.04077625620098907], [-0.8701977133750916, 0.046391229463021155], [-0.87467360496521, 0.06100357457813728]]</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>[[0.09682933141436782], [0.04484456326497293], [0.06471362195628479], [0.07555854266449227], [0.0020063520475156154], [0.0017380186186091058], [0.0020175598447174717], [0.007683141151680322], [0.0035923654630059766], [0.004749775194149533]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Equalized Odds_Sex_(0.1, 0.001)</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="n">
+        <v>50</v>
+      </c>
+      <c r="D7" t="n">
+        <v>10</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Equalized Odds</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>[[-0.827468991279602, 0.017130816597831798], [-0.8325666189193726, 0.017652343921789805], [-0.873678982257843, 0.053017032418612706], [-0.8717725276947021, 0.052872753093839944], [-0.8573500514030457, 0.029213605668917265], [-0.8709851503372192, 0.04755957051568413], [-0.8675453066825867, 0.038641629445944244], [-0.8747150897979736, 0.05932383918796201], [-0.8682084083557129, 0.04502917862886291], [-0.870322048664093, 0.04622310933003728], [-0.8670479655265808, 0.035323204976170766], [-0.8680840730667114, 0.03884237316600017]]</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>[[0.09354873019997026], [0.04282993489942096], [0.0037368712036962327], [0.003045042301467457], [0.015863333177623326], [0.0044117923999603325], [0.006421912069214856], [0.0023306674900125295], [0.008211184477728109], [0.0035391265529110586], [0.0022594703768275], [0.0028852438209539294]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Equalized Odds_Sex_(0.1, 0.1)</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>50</v>
+      </c>
+      <c r="D8" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Equalized Odds</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>[[-0.8113058805465698, 0.0038624423943578296], [-0.7522483468055725, 0.0], [-0.8545318841934204, 0.031128971571315008], [-0.8268473744392395, 0.013927545546359568], [-0.8728915452957153, 0.07820543781316779], [-0.8726842999458313, 0.0695954469457147], [-0.8491027355194092, 0.030416396303671718], [-0.8675867319107056, 0.04959096425653327], [-0.871523916721344, 0.05735864419612626], [-0.8449168801307678, 0.022928890867478798], [-0.8309917449951172, 0.014313177691690257], [-0.8685813546180725, 0.05594056617675992], [-0.8670893907546997, 0.04955389141399139], [-0.7522483468055725, 0.0], [-0.8690786957740784, 0.057234232211529436], [-0.8642712235450745, 0.04092450899379702], [-0.8658875226974487, 0.04636166634647459]]</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>[[0.04197753198888916], [0.09888722278175882], [0.025911617547587713], [0.09639152664637879], [0.002191128408852173], [0.003202766149796566], [0.05392172478021459], [0.0073486046188346], [0.002716075199586803], [0.08476803490002455], [0.0854971295412364], [0.009476593674124225], [0.0068693597770245534], [0.09864504875280274], [0.005563915328170643], [0.009063145746052267], [0.008454763210457406]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Equalized Odds_Sex_(0.1, 10)</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>50</v>
+      </c>
+      <c r="D9" t="n">
+        <v>10</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F9" t="n">
+        <v>10</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Equalized Odds</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>[[-0.8649757504463196, 0.04477503098404929], [-0.8466575741767883, 0.012382355127226845], [-0.852957010269165, 0.03977071160569], [-0.8511334657669067, 0.037407526854342954], [-0.8740519881248474, 0.062413268451358195], [-0.7915785908699036, 0.00174017325349363], [-0.7522897720336914, 0.0], [-0.8496415019035339, 0.03253338034627552], [-0.8723942041397095, 0.047915202334393184], [-0.8547391295433044, 0.04292101594247961]]</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>[[0.0093246256174029], [0.0559131138617306], [0.07482738382920621], [0.06385154153284131], [0.0032632262195883633], [0.07630135625276781], [0.0957714771607889], [0.07293848032051037], [0.0037931358102265573], [0.0426691253901261]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Equalized Odds_Sex_(10, 0.001)</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>50</v>
+      </c>
+      <c r="D10" t="n">
+        <v>10</v>
+      </c>
+      <c r="E10" t="n">
+        <v>10</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Equalized Odds</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>[[-0.8726428747177124, 0.06042160939086092], [-0.8716896772384644, 0.05664960518644309], [-0.8733474016189575, 0.06942911423039069], [-0.8735132217407227, 0.08096792395425137], [-0.8720626831054688, 0.05704095964010924], [-0.8726842999458313, 0.06122462284844422], [-0.8413112759590149, 0.0235051337464197], [-0.8704878091812134, 0.0531824907137866], [-0.871068000793457, 0.0558937975578474], [-0.8682498335838318, 0.04191900760514067], [-0.8651829957962036, 0.03301386135965646], [-0.8705706596374512, 0.05532550161497687], [-0.870114803314209, 0.044261887806236716]]</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>[[0.005093325405927208], [0.0028302062756110184], [0.0024905725950376124], [0.0035286209471135487], [0.002497101155402906], [0.004897714939421236], [0.04562392099360847], [0.0021665057698880864], [0.0019173170353772697], [0.004686199290776381], [0.006672207718285134], [0.0017491870607448392], [0.0029005544630838808]]</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testes 24 a 26
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,7 +483,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Equal Opportunity_Race_(10, 0.1)</t>
+          <t>Equalized Odds_Sex_(10, 0.1)</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -503,29 +503,29 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Equal Opportunity</t>
+          <t>Equalized Odds</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Race</t>
+          <t>Sex</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>[[-0.8735132217407227, 0.01620968150286095], [-0.8735546469688416, 0.02065927388728539], [-0.8723527789115906, 0.00232416831231963], [-0.8702805638313293, 0.00029621753000153017], [-0.8640225529670715, 0.00021140310901823778]]</t>
+          <t>[[-0.8258526921272278, 0.006683141771024852], [-0.8726014494895935, 0.07748801465733918], [-0.8457872271537781, 0.03125958165168193], [-0.8389489650726318, 0.010626288001592467], [-0.8718554377555847, 0.05476205356029165], [-0.8499315977096558, 0.03311049764536657], [-0.752372682094574, 0.0], [-0.8621990084648132, 0.03850044916905654], [-0.872477114200592, 0.06526134489419645], [-0.7946040034294128, 0.00012707382240681052], [-0.8402751684188843, 0.017449375573998963], [-0.869907557964325, 0.04349638440127038]]</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>[[0.0028737239939516388], [0.002971458386903831], [0.0028684319319696016], [0.00374261365951772], [0.003322649616601183]]</t>
+          <t>[[0.0720604168948716], [0.002836020560472824], [0.0421904887623584], [0.06813019151383098], [0.0027850457024521805], [0.0649615009819186], [0.03772704255796117], [0.014769201910509478], [0.0034135680479825195], [0.07799149240476415], [0.06843056619169122], [0.0023400581311345883]]</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Equal Opportunity_Race_(10, 10)</t>
+          <t>Equalized Odds_Sex_(10, 10)</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -545,316 +545,22 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Equal Opportunity</t>
+          <t>Equalized Odds</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Race</t>
+          <t>Sex</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>[[-0.8714824318885803, 0.0001000050635474592], [-0.7522483468055725, 0.0], [-0.7522483468055725, 0.0], [-0.7522483468055725, 0.0], [-0.8719383478164673, 0.003046989720998483], [-0.8716482520103455, 0.0007949769608587287], [-0.8737204074859619, 0.02342143906020555], [-0.8714410066604614, 4.430604081229195e-05], [-0.8734303116798401, 0.009865056458554844]]</t>
+          <t>[[-0.7522483468055725, 0.0], [-0.8542832136154175, 0.03470551715393729], [-0.8537030220031738, 0.028834608829431747], [-0.7522483468055725, 0.0], [-0.8375813364982605, 0.019613565445590363], [-0.8352604508399963, 0.009348991626398333], [-0.8675453066825867, 0.0492088683691627], [-0.8714410066604614, 0.05365371316087197], [-0.7522483468055725, 0.0], [-0.8638982176780701, 0.04269289515625246], [-0.8387417793273926, 0.023556313043442474], [-0.7522483468055725, 0.0], [-0.8730158805847168, 0.07101133891470571], [-0.8401508331298828, 0.028692991342468964], [-0.7522483468055725, 0.0], [-0.8055452108383179, 0.00308148232732581], [-0.8608728051185608, 0.03868708643463157], [-0.7522483468055725, 0.0], [-0.8399022221565247, 0.025090856111335286]]</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>[[0.0017745076722178134], [0.09895409459406464], [0.0936968270797161], [0.0993825068792214], [0.0036615332415286], [0.0019053222938458059], [0.003641574953726978], [0.0034821088280922443], [0.0026614375568086764]]</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>Equalized Odds_Sex_(0.001, 0.001)</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="n">
-        <v>50</v>
-      </c>
-      <c r="D4" t="n">
-        <v>10</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Equalized Odds</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Sex</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>[[-0.8265987038612366, 0.02434565725661994], [-0.8366281390190125, 0.02605185671545674], [-0.8205893039703369, 0.00926165248434338], [-0.861991822719574, 0.03561748593405175], [-0.8743835091590881, 0.06744981278407403], [-0.8514236211776733, 0.029490282491716795], [-0.8687471747398376, 0.048114197214148835], [-0.8671308159828186, 0.03816643353082369], [-0.8685813546180725, 0.044599439702429675], [-0.8725599646568298, 0.05690462725140685], [-0.872477114200592, 0.04852629342814105]]</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>[[0.08947120568403436], [0.06863962454533037], [0.08972192871631018], [0.01608495754267763], [0.0030164253919121643], [0.02642312346147711], [0.0037476388128512305], [0.004986735525391881], [0.0030047753910134724], [0.0031146051421806842], [0.002996645218538682]]</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Equalized Odds_Sex_(0.001, 0.1)</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="n">
-        <v>50</v>
-      </c>
-      <c r="D5" t="n">
-        <v>10</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Equalized Odds</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Sex</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>[[-0.8409797549247742, 0.019156886663060965], [-0.8720211982727051, 0.05518519575823929], [-0.8688715100288391, 0.043365337110828385], [-0.8549463152885437, 0.03789376875341892], [-0.8682084083557129, 0.04321708431802043], [-0.873927652835846, 0.07447845338736221], [-0.8671723008155823, 0.042677477071546344], [-0.8717311024665833, 0.0481274292484796], [-0.8742177486419678, 0.07482657548007596], [-0.8735132217407227, 0.05616074002691672], [-0.8726014494895935, 0.05576672373544059], [-0.8738861680030823, 0.0658587667435385]]</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>[[0.06011712596813006], [0.0023875984547754884], [0.001859066934291876], [0.03252023115285509], [0.009259553645886206], [0.004570539122095032], [0.0026936556435444344], [0.0031369506917890535], [0.002748609887659027], [0.004064160090213528], [0.004228466779856352], [0.004137777386298756]]</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Equalized Odds_Sex_(0.001, 10)</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="n">
-        <v>50</v>
-      </c>
-      <c r="D6" t="n">
-        <v>10</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="F6" t="n">
-        <v>10</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Equalized Odds</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Sex</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>[[-0.7573459148406982, 0.0], [-0.8416428565979004, 0.02097208002178849], [-0.8485639691352844, 0.03869590779085207], [-0.8467819094657898, 0.02719901879771859], [-0.8742591738700867, 0.05169646510510659], [-0.8656388521194458, 0.03961320024658648], [-0.8704878091812134, 0.05025764532541417], [-0.8675453066825867, 0.04077625620098907], [-0.8701977133750916, 0.046391229463021155], [-0.87467360496521, 0.06100357457813728]]</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>[[0.09682933141436782], [0.04484456326497293], [0.06471362195628479], [0.07555854266449227], [0.0020063520475156154], [0.0017380186186091058], [0.0020175598447174717], [0.007683141151680322], [0.0035923654630059766], [0.004749775194149533]]</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Equalized Odds_Sex_(0.1, 0.001)</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" t="n">
-        <v>50</v>
-      </c>
-      <c r="D7" t="n">
-        <v>10</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Equalized Odds</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Sex</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>[[-0.827468991279602, 0.017130816597831798], [-0.8325666189193726, 0.017652343921789805], [-0.873678982257843, 0.053017032418612706], [-0.8717725276947021, 0.052872753093839944], [-0.8573500514030457, 0.029213605668917265], [-0.8709851503372192, 0.04755957051568413], [-0.8675453066825867, 0.038641629445944244], [-0.8747150897979736, 0.05932383918796201], [-0.8682084083557129, 0.04502917862886291], [-0.870322048664093, 0.04622310933003728], [-0.8670479655265808, 0.035323204976170766], [-0.8680840730667114, 0.03884237316600017]]</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>[[0.09354873019997026], [0.04282993489942096], [0.0037368712036962327], [0.003045042301467457], [0.015863333177623326], [0.0044117923999603325], [0.006421912069214856], [0.0023306674900125295], [0.008211184477728109], [0.0035391265529110586], [0.0022594703768275], [0.0028852438209539294]]</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Equalized Odds_Sex_(0.1, 0.1)</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="n">
-        <v>50</v>
-      </c>
-      <c r="D8" t="n">
-        <v>10</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Equalized Odds</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>Sex</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>[[-0.8113058805465698, 0.0038624423943578296], [-0.7522483468055725, 0.0], [-0.8545318841934204, 0.031128971571315008], [-0.8268473744392395, 0.013927545546359568], [-0.8728915452957153, 0.07820543781316779], [-0.8726842999458313, 0.0695954469457147], [-0.8491027355194092, 0.030416396303671718], [-0.8675867319107056, 0.04959096425653327], [-0.871523916721344, 0.05735864419612626], [-0.8449168801307678, 0.022928890867478798], [-0.8309917449951172, 0.014313177691690257], [-0.8685813546180725, 0.05594056617675992], [-0.8670893907546997, 0.04955389141399139], [-0.7522483468055725, 0.0], [-0.8690786957740784, 0.057234232211529436], [-0.8642712235450745, 0.04092450899379702], [-0.8658875226974487, 0.04636166634647459]]</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>[[0.04197753198888916], [0.09888722278175882], [0.025911617547587713], [0.09639152664637879], [0.002191128408852173], [0.003202766149796566], [0.05392172478021459], [0.0073486046188346], [0.002716075199586803], [0.08476803490002455], [0.0854971295412364], [0.009476593674124225], [0.0068693597770245534], [0.09864504875280274], [0.005563915328170643], [0.009063145746052267], [0.008454763210457406]]</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>Equalized Odds_Sex_(0.1, 10)</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" t="n">
-        <v>50</v>
-      </c>
-      <c r="D9" t="n">
-        <v>10</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F9" t="n">
-        <v>10</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Equalized Odds</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Sex</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>[[-0.8649757504463196, 0.04477503098404929], [-0.8466575741767883, 0.012382355127226845], [-0.852957010269165, 0.03977071160569], [-0.8511334657669067, 0.037407526854342954], [-0.8740519881248474, 0.062413268451358195], [-0.7915785908699036, 0.00174017325349363], [-0.7522897720336914, 0.0], [-0.8496415019035339, 0.03253338034627552], [-0.8723942041397095, 0.047915202334393184], [-0.8547391295433044, 0.04292101594247961]]</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>[[0.0093246256174029], [0.0559131138617306], [0.07482738382920621], [0.06385154153284131], [0.0032632262195883633], [0.07630135625276781], [0.0957714771607889], [0.07293848032051037], [0.0037931358102265573], [0.0426691253901261]]</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>Equalized Odds_Sex_(10, 0.001)</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" t="n">
-        <v>50</v>
-      </c>
-      <c r="D10" t="n">
-        <v>10</v>
-      </c>
-      <c r="E10" t="n">
-        <v>10</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Equalized Odds</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Sex</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>[[-0.8726428747177124, 0.06042160939086092], [-0.8716896772384644, 0.05664960518644309], [-0.8733474016189575, 0.06942911423039069], [-0.8735132217407227, 0.08096792395425137], [-0.8720626831054688, 0.05704095964010924], [-0.8726842999458313, 0.06122462284844422], [-0.8413112759590149, 0.0235051337464197], [-0.8704878091812134, 0.0531824907137866], [-0.871068000793457, 0.0558937975578474], [-0.8682498335838318, 0.04191900760514067], [-0.8651829957962036, 0.03301386135965646], [-0.8705706596374512, 0.05532550161497687], [-0.870114803314209, 0.044261887806236716]]</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>[[0.005093325405927208], [0.0028302062756110184], [0.0024905725950376124], [0.0035286209471135487], [0.002497101155402906], [0.004897714939421236], [0.04562392099360847], [0.0021665057698880864], [0.0019173170353772697], [0.004686199290776381], [0.006672207718285134], [0.0017491870607448392], [0.0029005544630838808]]</t>
+          <t>[[0.08782393189545545], [0.017066058914500432], [0.04162967372417659], [0.07577576340821449], [0.07617841240083235], [0.09296948390164726], [0.008057047556820914], [0.006016119795329136], [0.09103986047624911], [0.01277561454241902], [0.08836292858453894], [0.09123925139880788], [0.002240117548971489], [0.09932110870392455], [0.09246524167436099], [0.0855823463652505], [0.020837874015763706], [0.08969255518681019], [0.08849216840664628]]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
testes 27 a 32
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,7 +483,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Equalized Odds_Sex_(10, 0.1)</t>
+          <t>Equalized Odds_Race_(0.001, 0.001)</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -496,10 +496,10 @@
         <v>10</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>0.001</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1</v>
+        <v>0.001</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -508,24 +508,24 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Sex</t>
+          <t>Race</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>[[-0.8258526921272278, 0.006683141771024852], [-0.8726014494895935, 0.07748801465733918], [-0.8457872271537781, 0.03125958165168193], [-0.8389489650726318, 0.010626288001592467], [-0.8718554377555847, 0.05476205356029165], [-0.8499315977096558, 0.03311049764536657], [-0.752372682094574, 0.0], [-0.8621990084648132, 0.03850044916905654], [-0.872477114200592, 0.06526134489419645], [-0.7946040034294128, 0.00012707382240681052], [-0.8402751684188843, 0.017449375573998963], [-0.869907557964325, 0.04349638440127038]]</t>
+          <t>[[-0.8242363929748535, 0.014159401248010444], [-0.8745492696762085, 0.04942125245736562], [-0.8483567237854004, 0.022308763410192875], [-0.8272618055343628, 0.015153982078193153], [-0.8723942041397095, 0.041401527976946725], [-0.8729329705238342, 0.04163277990565041], [-0.8464503288269043, 0.019675899769046053], [-0.8696174621582031, 0.025799807076898284], [-0.873927652835846, 0.048502003441224226], [-0.8731402158737183, 0.043939038281920376], [-0.8715653419494629, 0.02747662629584531], [-0.872269868850708, 0.031295781863708405], [-0.8646027445793152, 0.024152517929055446]]</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>[[0.0720604168948716], [0.002836020560472824], [0.0421904887623584], [0.06813019151383098], [0.0027850457024521805], [0.0649615009819186], [0.03772704255796117], [0.014769201910509478], [0.0034135680479825195], [0.07799149240476415], [0.06843056619169122], [0.0023400581311345883]]</t>
+          <t>[[0.0720604168948716], [0.002836020560472824], [0.0559131138617306], [0.08765127631437424], [0.0057057463996129515], [0.002577534814659025], [0.030659470640097105], [0.0028352034648014795], [0.003095331604070015], [0.005586780177463361], [0.001933568534453362], [0.0035356390842225284], [0.004155429204476469]]</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Equalized Odds_Sex_(10, 10)</t>
+          <t>Equalized Odds_Race_(0.001, 0.1)</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -538,29 +538,197 @@
         <v>10</v>
       </c>
       <c r="E3" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Equalized Odds</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Race</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>[[-0.8729329705238342, 0.03932652152938046], [-0.8735546469688416, 0.04492886483761692], [-0.8708608150482178, 0.02273396964944826], [-0.8726842999458313, 0.039115291122808635], [-0.8721041083335876, 0.034613394954087606], [-0.8681669235229492, 0.02031283862696687]]</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>[[0.004001572844964948], [0.002443965282760008], [0.003986077195804353], [0.0018077342267215526], [0.0039166856703735506], [0.001969444193204859]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Equalized Odds_Race_(0.001, 10)</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>50</v>
+      </c>
+      <c r="D4" t="n">
         <v>10</v>
       </c>
-      <c r="F3" t="n">
+      <c r="E4" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F4" t="n">
         <v>10</v>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>Equalized Odds</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Sex</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>[[-0.7522483468055725, 0.0], [-0.8542832136154175, 0.03470551715393729], [-0.8537030220031738, 0.028834608829431747], [-0.7522483468055725, 0.0], [-0.8375813364982605, 0.019613565445590363], [-0.8352604508399963, 0.009348991626398333], [-0.8675453066825867, 0.0492088683691627], [-0.8714410066604614, 0.05365371316087197], [-0.7522483468055725, 0.0], [-0.8638982176780701, 0.04269289515625246], [-0.8387417793273926, 0.023556313043442474], [-0.7522483468055725, 0.0], [-0.8730158805847168, 0.07101133891470571], [-0.8401508331298828, 0.028692991342468964], [-0.7522483468055725, 0.0], [-0.8055452108383179, 0.00308148232732581], [-0.8608728051185608, 0.03868708643463157], [-0.7522483468055725, 0.0], [-0.8399022221565247, 0.025090856111335286]]</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>[[0.08782393189545545], [0.017066058914500432], [0.04162967372417659], [0.07577576340821449], [0.07617841240083235], [0.09296948390164726], [0.008057047556820914], [0.006016119795329136], [0.09103986047624911], [0.01277561454241902], [0.08836292858453894], [0.09123925139880788], [0.002240117548971489], [0.09932110870392455], [0.09246524167436099], [0.0855823463652505], [0.020837874015763706], [0.08969255518681019], [0.08849216840664628]]</t>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Race</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>[[-0.8619089126586914, 0.02549898203282666], [-0.8486883044242859, 0.02446810800867916], [-0.8347631692886353, 0.021626022809334945], [-0.872725784778595, 0.043879475927618386], [-0.8736375570297241, 0.04493837338658924], [-0.8678354024887085, 0.03005042979478375], [-0.8674623966217041, 0.02795540182508562], [-0.8722284436225891, 0.035812945280075156], [-0.8711509108543396, 0.03206587388804802], [-0.8726428747177124, 0.03783364585991919], [-0.8707779049873352, 0.030407067342858418], [-0.8629035353660583, 0.025808813413777], [-0.874880850315094, 0.05666187857656621], [-0.8680840730667114, 0.030337494227490495], [-0.8720211982727051, 0.03211967754367664]]</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>[[0.009924848699921704], [0.07503941706300225], [0.09086869075900025], [0.004273323343272307], [0.0023895398211110945], [0.007803082023880141], [0.0026085558453432882], [0.006096653228117211], [0.0028502520542225845], [0.004606693194367068], [0.0038426154255498304], [0.010921646514229267], [0.0026291574446831944], [0.0032930808050942997], [0.005800639842243884]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Equalized Odds_Race_(0.1, 0.001)</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>50</v>
+      </c>
+      <c r="D5" t="n">
+        <v>10</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Equalized Odds</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Race</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>[[-0.7633967399597168, 0.00013064210595074792], [-0.8711094260215759, 0.030486149007198676], [-0.872477114200592, 0.036467662446109717], [-0.8698247075080872, 0.02036614007050188], [-0.8718968629837036, 0.03514071765237675], [-0.8382444381713867, 0.014053534938677725], [-0.8739690780639648, 0.04636592800307515], [-0.8725599646568298, 0.042753248567297716]]</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>[[0.08947120568403436], [0.0026459700330397585], [0.0038954644340870328], [0.004816235113004338], [0.00408031450697115], [0.03952480124322402], [0.002516430643276443], [0.0045271594241939675]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Equalized Odds_Race_(0.1, 0.1)</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>50</v>
+      </c>
+      <c r="D6" t="n">
+        <v>10</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Equalized Odds</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Race</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>[[-0.8728086352348328, 0.04566792015457151], [-0.7522483468055725, 0.0], [-0.8678354024887085, 0.03050767716561137], [-0.8716482520103455, 0.04253250961175356], [-0.8700318932533264, 0.0363622983488706], [-0.8728915452957153, 0.051737521594701505], [-0.8711509108543396, 0.040335867395115264], [-0.8417671918869019, 0.016279205014326607], [-0.8359235525131226, 0.010279678901658134], [-0.8548219799995422, 0.021896313358115156], [-0.8480252027511597, 0.021207311846490235], [-0.8722284436225891, 0.04377310740619205], [-0.8682498335838318, 0.035663286076179745], [-0.8658460974693298, 0.0295083420609425], [-0.8568941950798035, 0.02469360123870948], [-0.8636495471000671, 0.028323054558413448]]</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>[[0.002836020560472824], [0.09395666529574745], [0.005660977500076756], [0.004329113995310084], [0.00421014211672947], [0.003668268240272974], [0.0025752790440976845], [0.054385473424672974], [0.058182731619724815], [0.024883423091979016], [0.061338221654791414], [0.004347405255735161], [0.009440373292847835], [0.005123701552146722], [0.03253262230350703], [0.003970822547819292]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Equalized Odds_Race_(0.1, 10)</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="n">
+        <v>50</v>
+      </c>
+      <c r="D7" t="n">
+        <v>10</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>10</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Equalized Odds</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Race</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>[[-0.7522483468055725, 0.0], [-0.8494343161582947, 0.001698615223809652], [-0.8671723008155823, 0.021765169040070798], [-0.8713995814323425, 0.035994645615542775], [-0.8741348385810852, 0.050330490712441084], [-0.8708608150482178, 0.032723838692287927], [-0.7522483468055725, 0.0], [-0.850801944732666, 0.01444244798396832], [-0.8734303116798401, 0.04998912041201213]]</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>[[0.09579316406203515], [0.028936015992545895], [0.003589614050798086], [0.0031183331037854603], [0.002759758366152665], [0.002694870587713256], [0.09548765190984926], [0.06725469668650612], [0.002166291379806841]]</t>
         </is>
       </c>
     </row>

</xml_diff>